<commit_message>
Final Commit for Branch creation
</commit_message>
<xml_diff>
--- a/cucumberframework/InputExcelData/Measurement.xlsx
+++ b/cucumberframework/InputExcelData/Measurement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\git\TouchPointFramework\TouchPointFramework\cucumberframework\InputExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FF13CBC-57AE-4DF6-9971-84615B3F0ECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9455049-9C8F-4A16-851F-3D924C28971A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Room</t>
   </si>
@@ -133,6 +133,21 @@
   </si>
   <si>
     <t>Entertainment</t>
+  </si>
+  <si>
+    <t>ImageName</t>
+  </si>
+  <si>
+    <t>communication log.png</t>
+  </si>
+  <si>
+    <t>camp.png</t>
+  </si>
+  <si>
+    <t>Before edit.png</t>
+  </si>
+  <si>
+    <t>After edit.png</t>
   </si>
 </sst>
 </file>
@@ -485,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -497,10 +512,12 @@
     <col min="2" max="2" width="19.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="12" width="8.88671875" style="1"/>
+    <col min="13" max="13" width="13.77734375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -537,8 +554,11 @@
       <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="M1" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -575,8 +595,11 @@
       <c r="L2" s="1">
         <v>54</v>
       </c>
+      <c r="M2" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
@@ -613,8 +636,11 @@
       <c r="L3" s="1">
         <v>53</v>
       </c>
+      <c r="M3" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
@@ -651,8 +677,11 @@
       <c r="L4" s="1">
         <v>52</v>
       </c>
+      <c r="M4" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>25</v>
       </c>
@@ -688,6 +717,9 @@
       </c>
       <c r="L5" s="1">
         <v>51</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>